<commit_message>
add investigation file reader references #26
</commit_message>
<xml_diff>
--- a/tests/ArcCommander.Tests.NetCore/ArcCommander/TestFiles/isa.investigation.xlsx
+++ b/tests/ArcCommander.Tests.NetCore/ArcCommander/TestFiles/isa.investigation.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\arcCommander\tests\ArcCommander.Tests.NetCore\ArcCommander\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{14B01E20-7DF4-4805-A9E5-E6CC3D038964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{71B8F4F6-55DF-4CEF-AA04-0995D46D2668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40590" yWindow="3750" windowWidth="21600" windowHeight="12540"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Text Document" sheetId="1" r:id="rId1"/>
@@ -498,15 +498,9 @@
     <t>sample volume;standard volume</t>
   </si>
   <si>
-    <t>Study Protocol Parameters Name Term Accession Number</t>
-  </si>
-  <si>
     <t>;</t>
   </si>
   <si>
-    <t>Study Protocol Parameters Name Term Source REF</t>
-  </si>
-  <si>
     <t>Study Protocol Components Name</t>
   </si>
   <si>
@@ -607,12 +601,18 @@
   </si>
   <si>
     <t>This was done using Enzo BioArrayTM HighYieldTM RNA transcript labelling kit (T7) with 5 ul cDNA. The resultant cRNA was again purified using the GeneChip Sample Clean Up Module. The column was eluted in the first instance using 10 l RNase-free water, and for a second time using 11 l RNase-free water. cRNA was quantified using the Nanodrop spectrophotometer. A total of 15 ug of cRNA (required for hybridisation) was fragmented. Fragmentation was carried out by using 2 ul of fragmentation buffer for every 8 ul cRNA.</t>
+  </si>
+  <si>
+    <t>Study Protocol Parameters Term Accession Number</t>
+  </si>
+  <si>
+    <t>Study Protocol Parameters Term Source REF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1447,21 +1447,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="E132" sqref="E132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="43.53515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1487,7 +1490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1498,7 +1501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1524,7 +1527,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1550,12 +1553,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1563,7 +1566,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1571,7 +1574,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1587,7 +1590,7 @@
         <v>2007-04-30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1595,12 +1598,12 @@
         <v>2009-03-10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1608,12 +1611,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>17439666</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1629,7 +1632,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1653,22 +1656,22 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1682,7 +1685,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -1696,7 +1699,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1710,22 +1713,22 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -1739,7 +1742,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -1753,7 +1756,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -1767,27 +1770,27 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -1795,7 +1798,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -1803,7 +1806,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -1811,17 +1814,17 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -1829,7 +1832,7 @@
         <v>2007-04-30</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -1837,7 +1840,7 @@
         <v>2009-03-10</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -1845,12 +1848,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -1858,7 +1861,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -1866,7 +1869,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>89</v>
       </c>
@@ -1874,12 +1877,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>91</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>17439666</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>92</v>
       </c>
@@ -1895,7 +1898,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>93</v>
       </c>
@@ -1903,7 +1906,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>94</v>
       </c>
@@ -1911,7 +1914,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>95</v>
       </c>
@@ -1919,22 +1922,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>100</v>
       </c>
@@ -1945,7 +1948,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>103</v>
       </c>
@@ -1956,7 +1959,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>105</v>
       </c>
@@ -1964,7 +1967,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>107</v>
       </c>
@@ -1972,12 +1975,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>109</v>
       </c>
@@ -1991,7 +1994,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>113</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>116</v>
       </c>
@@ -2019,7 +2022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>117</v>
       </c>
@@ -2033,7 +2036,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>120</v>
       </c>
@@ -2041,7 +2044,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>122</v>
       </c>
@@ -2055,7 +2058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>123</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>127</v>
       </c>
@@ -2083,12 +2086,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>132</v>
       </c>
@@ -2114,7 +2117,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -2140,7 +2143,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>145</v>
       </c>
@@ -2148,7 +2151,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>147</v>
       </c>
@@ -2156,7 +2159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>148</v>
       </c>
@@ -2173,17 +2176,17 @@
         <v>152</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>155</v>
       </c>
@@ -2191,50 +2194,50 @@
         <v>156</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
+        <v>192</v>
+      </c>
+      <c r="H79" t="s">
         <v>157</v>
       </c>
-      <c r="H79" t="s">
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A80" t="s">
+        <v>193</v>
+      </c>
+      <c r="H80" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A81" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A82" t="s">
         <v>159</v>
       </c>
-      <c r="H80" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A85" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>165</v>
       </c>
       <c r="B86" t="s">
         <v>51</v>
@@ -2246,9 +2249,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B87" t="s">
         <v>47</v>
@@ -2260,9 +2263,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B88" t="s">
         <v>55</v>
@@ -2274,24 +2277,24 @@
         <v>57</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A90" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>171</v>
       </c>
       <c r="B92" t="s">
         <v>62</v>
@@ -2303,9 +2306,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B93" t="s">
         <v>64</v>
@@ -2317,9 +2320,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B94" t="s">
         <v>66</v>
@@ -2331,61 +2334,61 @@
         <v>67</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A96" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A97" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>72</v>
       </c>
       <c r="B99" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>74</v>
       </c>
       <c r="B100" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
         <v>76</v>
       </c>
       <c r="B101" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
         <v>80</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>2007-04-30</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
         <v>81</v>
       </c>
@@ -2401,36 +2404,36 @@
         <v>2009-03-10</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
         <v>82</v>
       </c>
       <c r="B106" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
         <v>85</v>
       </c>
       <c r="B108" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
         <v>87</v>
       </c>
       <c r="B109" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
         <v>89</v>
       </c>
@@ -2438,12 +2441,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
         <v>91</v>
       </c>
@@ -2451,17 +2454,17 @@
         <v>17439666</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
         <v>94</v>
       </c>
@@ -2469,7 +2472,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
         <v>95</v>
       </c>
@@ -2477,61 +2480,61 @@
         <v>42</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A118" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A119" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
         <v>100</v>
       </c>
       <c r="B120" t="s">
+        <v>181</v>
+      </c>
+      <c r="C120" t="s">
+        <v>182</v>
+      </c>
+      <c r="D120" t="s">
         <v>183</v>
       </c>
-      <c r="C120" t="s">
-        <v>184</v>
-      </c>
-      <c r="D120" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A121" t="s">
         <v>103</v>
       </c>
       <c r="B121" t="s">
+        <v>181</v>
+      </c>
+      <c r="C121" t="s">
+        <v>184</v>
+      </c>
+      <c r="D121" t="s">
         <v>183</v>
       </c>
-      <c r="C121" t="s">
-        <v>186</v>
-      </c>
-      <c r="D121" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A122" t="s">
         <v>105</v>
       </c>
       <c r="C122" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D122" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A123" t="s">
         <v>107</v>
       </c>
@@ -2542,12 +2545,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A124" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
         <v>109</v>
       </c>
@@ -2555,7 +2558,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
         <v>113</v>
       </c>
@@ -2563,7 +2566,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
         <v>116</v>
       </c>
@@ -2571,7 +2574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
         <v>117</v>
       </c>
@@ -2579,7 +2582,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>120</v>
       </c>
@@ -2587,7 +2590,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
         <v>122</v>
       </c>
@@ -2595,7 +2598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
         <v>123</v>
       </c>
@@ -2603,20 +2606,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
         <v>127</v>
       </c>
       <c r="B132" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A133" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A134" t="s">
         <v>132</v>
       </c>
@@ -2633,7 +2636,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A135" t="s">
         <v>140</v>
       </c>
@@ -2650,86 +2653,86 @@
         <v>142</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A136" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A137" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A138" t="s">
         <v>148</v>
       </c>
       <c r="B138" t="s">
+        <v>188</v>
+      </c>
+      <c r="C138" t="s">
+        <v>189</v>
+      </c>
+      <c r="D138" t="s">
         <v>190</v>
       </c>
-      <c r="C138" t="s">
+      <c r="E138" t="s">
         <v>191</v>
       </c>
-      <c r="D138" t="s">
-        <v>192</v>
-      </c>
-      <c r="E138" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A139" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A143" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A144" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A145" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A146" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A147" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A148" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A149" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>165</v>
       </c>
       <c r="B149" t="s">
         <v>51</v>
@@ -2741,9 +2744,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A150" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B150" t="s">
         <v>47</v>
@@ -2755,9 +2758,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A151" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B151" t="s">
         <v>55</v>
@@ -2769,24 +2772,24 @@
         <v>57</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A152" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A153" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A154" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A155" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>171</v>
       </c>
       <c r="B155" t="s">
         <v>62</v>
@@ -2798,9 +2801,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A156" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B156" t="s">
         <v>64</v>
@@ -2812,9 +2815,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A157" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B157" t="s">
         <v>66</v>
@@ -2826,19 +2829,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A158" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A159" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A160" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add IsaXLSX IO tests
</commit_message>
<xml_diff>
--- a/tests/ArcCommander.Tests.NetCore/ArcCommander/TestFiles/isa.investigation.xlsx
+++ b/tests/ArcCommander.Tests.NetCore/ArcCommander/TestFiles/isa.investigation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\arcCommander\tests\ArcCommander.Tests.NetCore\ArcCommander\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{71B8F4F6-55DF-4CEF-AA04-0995D46D2668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6020251A-48AB-43C8-A088-7EA533E0582E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44880" yWindow="4230" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Text Document" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="343" uniqueCount="194">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="348" uniqueCount="199">
   <si>
     <t>ONTOLOGY SOURCE REFERENCE</t>
   </si>
@@ -117,21 +117,12 @@
     <t>Investigation Public Release Date</t>
   </si>
   <si>
-    <t>Comment[Created With Configuration]</t>
-  </si>
-  <si>
-    <t>Comment[Last Opened With Configuration]</t>
-  </si>
-  <si>
     <t>isaconfig-default_v2013-02-13</t>
   </si>
   <si>
     <t>INVESTIGATION PUBLICATIONS</t>
   </si>
   <si>
-    <t>Investigation PubMed ID</t>
-  </si>
-  <si>
     <t>Investigation Publication DOI</t>
   </si>
   <si>
@@ -237,9 +228,6 @@
     <t>Investigation Person Roles Term Source REF</t>
   </si>
   <si>
-    <t>Comment[Investigation Person REF]</t>
-  </si>
-  <si>
     <t>STUDY</t>
   </si>
   <si>
@@ -261,12 +249,6 @@
     <t>We wished to study the impact of growth rate on the total complement of mRNA molecules, proteins, and metabolites in S. cerevisiae, independent of any nutritional or other physiological effects. To achieve this, we carried out our analyses on yeast grown in steady-state chemostat culture under four different nutrient limitations (glucose, ammonium, phosphate, and sulfate) at three different dilution (that is, growth) rates (D = u = 0.07, 0.1, and 0.2/hour, equivalent to population doubling times (Td) of 10 hours, 7 hours, and 3.5 hours, respectively; u = specific growth rate defined as grams of biomass generated per gram of biomass present per unit time).</t>
   </si>
   <si>
-    <t>Comment[Study Grant Number]</t>
-  </si>
-  <si>
-    <t>Comment[Study Funding Agency]</t>
-  </si>
-  <si>
     <t>Study Submission Date</t>
   </si>
   <si>
@@ -300,9 +282,6 @@
     <t>STUDY PUBLICATIONS</t>
   </si>
   <si>
-    <t>Study PubMed ID</t>
-  </si>
-  <si>
     <t>Study Publication DOI</t>
   </si>
   <si>
@@ -549,9 +528,6 @@
     <t>Study Person Roles Term Source REF</t>
   </si>
   <si>
-    <t>Comment[Study Person REF]</t>
-  </si>
-  <si>
     <t>BII-S-2</t>
   </si>
   <si>
@@ -607,6 +583,45 @@
   </si>
   <si>
     <t>Study Protocol Parameters Term Source REF</t>
+  </si>
+  <si>
+    <t>Comment[&lt;Created With Configuration&gt;]</t>
+  </si>
+  <si>
+    <t>Comment[&lt;Last Opened With Configuration&gt;]</t>
+  </si>
+  <si>
+    <t>Comment[&lt;Investigation Person REF&gt;]</t>
+  </si>
+  <si>
+    <t>Comment[&lt;Study Grant Number&gt;]</t>
+  </si>
+  <si>
+    <t>Comment[&lt;Study Funding Agency&gt;]</t>
+  </si>
+  <si>
+    <t>Comment[&lt;Study Person REF&gt;]</t>
+  </si>
+  <si>
+    <t>#TestRemark1</t>
+  </si>
+  <si>
+    <t>#TestRemark2</t>
+  </si>
+  <si>
+    <t>#TestRemark3</t>
+  </si>
+  <si>
+    <t>#TestRemark4</t>
+  </si>
+  <si>
+    <t>#TestRemark5</t>
+  </si>
+  <si>
+    <t>Investigation Publication PubMed ID</t>
+  </si>
+  <si>
+    <t>Study Publication PubMed ID</t>
   </si>
 </sst>
 </file>
@@ -1448,10 +1463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H160"/>
+  <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1492,1107 +1507,1098 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>47893</v>
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>47893</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="d">
-        <v>2007-04-30</v>
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="d">
-        <v>2009-03-10</v>
+        <v>2007-04-30</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="d">
+        <v>2009-03-10</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>187</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15">
-        <v>17439666</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
+        <v>197</v>
+      </c>
+      <c r="B16">
+        <v>17439666</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D31" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>72</v>
+      </c>
+      <c r="B39" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>74</v>
+      </c>
+      <c r="B40" s="1" t="d">
+        <v>2007-04-30</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B41" s="1" t="d">
-        <v>2007-04-30</v>
+        <v>2009-03-10</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="1" t="d">
-        <v>2009-03-10</v>
+        <v>76</v>
+      </c>
+      <c r="B42" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" t="s">
-        <v>83</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>89</v>
-      </c>
-      <c r="B47" t="s">
-        <v>2</v>
+        <v>193</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>81</v>
+      </c>
+      <c r="B48" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>91</v>
-      </c>
-      <c r="B49">
-        <v>17439666</v>
+        <v>83</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>92</v>
-      </c>
-      <c r="B50" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>93</v>
-      </c>
-      <c r="B51" t="s">
-        <v>38</v>
+        <v>198</v>
+      </c>
+      <c r="B51">
+        <v>17439666</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B52" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B53" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>97</v>
+        <v>87</v>
+      </c>
+      <c r="B54" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
-        <v>98</v>
+        <v>88</v>
+      </c>
+      <c r="B55" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>100</v>
-      </c>
-      <c r="B57" t="s">
-        <v>101</v>
-      </c>
-      <c r="C57" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
-        <v>103</v>
-      </c>
-      <c r="B58" t="s">
-        <v>104</v>
-      </c>
-      <c r="C58" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>93</v>
+      </c>
+      <c r="B59" t="s">
+        <v>94</v>
       </c>
       <c r="C59" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>107</v>
+        <v>96</v>
+      </c>
+      <c r="B60" t="s">
+        <v>97</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
-        <v>108</v>
+        <v>98</v>
+      </c>
+      <c r="C61" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
-        <v>109</v>
-      </c>
-      <c r="B62" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>111</v>
-      </c>
-      <c r="D62" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
-        <v>113</v>
-      </c>
-      <c r="B63" t="s">
-        <v>114</v>
-      </c>
-      <c r="C63" t="s">
-        <v>115</v>
-      </c>
-      <c r="D63">
-        <v>424</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B64" t="s">
-        <v>2</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>2</v>
+        <v>104</v>
       </c>
       <c r="D64" t="s">
-        <v>2</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B65" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C65" t="s">
-        <v>118</v>
-      </c>
-      <c r="D65" t="s">
-        <v>119</v>
+        <v>108</v>
+      </c>
+      <c r="D65">
+        <v>424</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>120</v>
+        <v>109</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>121</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B67" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="C67" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="D67" t="s">
-        <v>2</v>
+        <v>112</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>123</v>
-      </c>
-      <c r="B68" t="s">
-        <v>124</v>
-      </c>
-      <c r="C68" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D68" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B69" t="s">
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>129</v>
+        <v>2</v>
       </c>
       <c r="D69" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>131</v>
+        <v>116</v>
+      </c>
+      <c r="B70" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70" t="s">
+        <v>118</v>
+      </c>
+      <c r="D70" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B71" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C71" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D71" t="s">
-        <v>135</v>
-      </c>
-      <c r="E71" t="s">
-        <v>136</v>
-      </c>
-      <c r="F71" t="s">
-        <v>137</v>
-      </c>
-      <c r="G71" t="s">
-        <v>138</v>
-      </c>
-      <c r="H71" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>140</v>
-      </c>
-      <c r="B72" t="s">
-        <v>141</v>
-      </c>
-      <c r="C72" t="s">
-        <v>134</v>
-      </c>
-      <c r="D72" t="s">
-        <v>135</v>
-      </c>
-      <c r="E72" t="s">
-        <v>142</v>
-      </c>
-      <c r="F72" t="s">
-        <v>142</v>
-      </c>
-      <c r="G72" t="s">
-        <v>143</v>
-      </c>
-      <c r="H72" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
-        <v>145</v>
+        <v>125</v>
+      </c>
+      <c r="B73" t="s">
+        <v>126</v>
+      </c>
+      <c r="C73" t="s">
+        <v>127</v>
+      </c>
+      <c r="D73" t="s">
+        <v>128</v>
+      </c>
+      <c r="E73" t="s">
+        <v>129</v>
+      </c>
+      <c r="F73" t="s">
+        <v>130</v>
+      </c>
+      <c r="G73" t="s">
+        <v>131</v>
       </c>
       <c r="H73" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>147</v>
+        <v>133</v>
+      </c>
+      <c r="B74" t="s">
+        <v>134</v>
+      </c>
+      <c r="C74" t="s">
+        <v>127</v>
+      </c>
+      <c r="D74" t="s">
+        <v>128</v>
+      </c>
+      <c r="E74" t="s">
+        <v>135</v>
+      </c>
+      <c r="F74" t="s">
+        <v>135</v>
+      </c>
+      <c r="G74" t="s">
+        <v>136</v>
       </c>
       <c r="H74" t="s">
-        <v>2</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
-        <v>148</v>
-      </c>
-      <c r="B75" t="s">
-        <v>149</v>
-      </c>
-      <c r="C75" t="s">
-        <v>150</v>
-      </c>
-      <c r="E75" t="s">
-        <v>151</v>
-      </c>
-      <c r="G75" t="s">
-        <v>152</v>
+        <v>138</v>
+      </c>
+      <c r="H75" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>153</v>
+        <v>140</v>
+      </c>
+      <c r="H76" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
-        <v>154</v>
+        <v>141</v>
+      </c>
+      <c r="B77" t="s">
+        <v>142</v>
+      </c>
+      <c r="C77" t="s">
+        <v>143</v>
+      </c>
+      <c r="E77" t="s">
+        <v>144</v>
+      </c>
+      <c r="G77" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
-        <v>155</v>
-      </c>
-      <c r="H78" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
-        <v>192</v>
-      </c>
-      <c r="H79" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
       <c r="H80" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A81" t="s">
+        <v>184</v>
+      </c>
+      <c r="H81" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A82" t="s">
+        <v>185</v>
+      </c>
+      <c r="H82" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A85" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A87" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A88" t="s">
+        <v>156</v>
+      </c>
+      <c r="B88" t="s">
+        <v>48</v>
+      </c>
+      <c r="C88" t="s">
+        <v>49</v>
+      </c>
+      <c r="D88" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A89" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A81" t="s">
+      <c r="B89" t="s">
+        <v>44</v>
+      </c>
+      <c r="C89" t="s">
+        <v>45</v>
+      </c>
+      <c r="D89" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A90" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A82" t="s">
+      <c r="B90" t="s">
+        <v>52</v>
+      </c>
+      <c r="C90" t="s">
+        <v>53</v>
+      </c>
+      <c r="D90" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A83" t="s">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A84" t="s">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A93" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A85" t="s">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A94" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A86" t="s">
+      <c r="B94" t="s">
+        <v>59</v>
+      </c>
+      <c r="C94" t="s">
+        <v>59</v>
+      </c>
+      <c r="D94" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A95" t="s">
         <v>163</v>
       </c>
-      <c r="B86" t="s">
-        <v>51</v>
-      </c>
-      <c r="C86" t="s">
-        <v>52</v>
-      </c>
-      <c r="D86" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A87" t="s">
+      <c r="B95" t="s">
+        <v>61</v>
+      </c>
+      <c r="C95" t="s">
+        <v>61</v>
+      </c>
+      <c r="D95" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A96" t="s">
         <v>164</v>
       </c>
-      <c r="B87" t="s">
-        <v>47</v>
-      </c>
-      <c r="C87" t="s">
-        <v>48</v>
-      </c>
-      <c r="D87" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A88" t="s">
-        <v>165</v>
-      </c>
-      <c r="B88" t="s">
-        <v>55</v>
-      </c>
-      <c r="C88" t="s">
-        <v>56</v>
-      </c>
-      <c r="D88" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A89" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A90" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A91" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A92" t="s">
-        <v>169</v>
-      </c>
-      <c r="B92" t="s">
-        <v>62</v>
-      </c>
-      <c r="C92" t="s">
-        <v>62</v>
-      </c>
-      <c r="D92" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A93" t="s">
-        <v>170</v>
-      </c>
-      <c r="B93" t="s">
+      <c r="B96" t="s">
+        <v>63</v>
+      </c>
+      <c r="C96" t="s">
         <v>64</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D96" t="s">
         <v>64</v>
-      </c>
-      <c r="D93" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A94" t="s">
-        <v>171</v>
-      </c>
-      <c r="B94" t="s">
-        <v>66</v>
-      </c>
-      <c r="C94" t="s">
-        <v>67</v>
-      </c>
-      <c r="D94" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A95" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A96" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
-        <v>71</v>
+        <v>166</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
-        <v>72</v>
-      </c>
-      <c r="B99" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
-        <v>74</v>
-      </c>
-      <c r="B100" t="s">
-        <v>176</v>
+        <v>67</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
-        <v>76</v>
-      </c>
-      <c r="B101" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
-        <v>78</v>
+        <v>68</v>
+      </c>
+      <c r="B102" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+      <c r="B103" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
-        <v>80</v>
-      </c>
-      <c r="B104" s="1" t="d">
-        <v>2007-04-30</v>
+        <v>72</v>
+      </c>
+      <c r="B104" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B105" s="1" t="d">
-        <v>2009-03-10</v>
+        <v>2007-04-30</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
-        <v>82</v>
-      </c>
-      <c r="B106" t="s">
-        <v>178</v>
+        <v>75</v>
+      </c>
+      <c r="B106" s="1" t="d">
+        <v>2009-03-10</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
-        <v>84</v>
+        <v>76</v>
+      </c>
+      <c r="B107" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
-        <v>85</v>
-      </c>
-      <c r="B108" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
-        <v>87</v>
-      </c>
-      <c r="B109" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
-        <v>89</v>
-      </c>
-      <c r="B110" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
-        <v>90</v>
+        <v>79</v>
+      </c>
+      <c r="B111" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
-        <v>91</v>
-      </c>
-      <c r="B112">
-        <v>17439666</v>
+        <v>81</v>
+      </c>
+      <c r="B112" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
-        <v>92</v>
+        <v>83</v>
+      </c>
+      <c r="B113" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
-        <v>94</v>
-      </c>
-      <c r="B115" t="s">
-        <v>40</v>
+        <v>198</v>
+      </c>
+      <c r="B115">
+        <v>17439666</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
-        <v>95</v>
-      </c>
-      <c r="B116" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A118" t="s">
-        <v>98</v>
+        <v>87</v>
+      </c>
+      <c r="B118" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A119" t="s">
-        <v>99</v>
+        <v>88</v>
+      </c>
+      <c r="B119" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
-        <v>100</v>
-      </c>
-      <c r="B120" t="s">
-        <v>181</v>
-      </c>
-      <c r="C120" t="s">
-        <v>182</v>
-      </c>
-      <c r="D120" t="s">
-        <v>183</v>
+        <v>90</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A121" t="s">
-        <v>103</v>
-      </c>
-      <c r="B121" t="s">
-        <v>181</v>
-      </c>
-      <c r="C121" t="s">
-        <v>184</v>
-      </c>
-      <c r="D121" t="s">
-        <v>183</v>
+        <v>91</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A122" t="s">
-        <v>105</v>
-      </c>
-      <c r="C122" t="s">
-        <v>185</v>
-      </c>
-      <c r="D122" t="s">
-        <v>186</v>
+        <v>92</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A123" t="s">
-        <v>107</v>
+        <v>93</v>
+      </c>
+      <c r="B123" t="s">
+        <v>173</v>
       </c>
       <c r="C123" t="s">
-        <v>8</v>
+        <v>174</v>
       </c>
       <c r="D123" t="s">
-        <v>8</v>
+        <v>175</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A124" t="s">
-        <v>108</v>
+        <v>96</v>
+      </c>
+      <c r="B124" t="s">
+        <v>173</v>
+      </c>
+      <c r="C124" t="s">
+        <v>176</v>
+      </c>
+      <c r="D124" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
-        <v>109</v>
-      </c>
-      <c r="B125" t="s">
-        <v>112</v>
+        <v>98</v>
+      </c>
+      <c r="C125" t="s">
+        <v>177</v>
+      </c>
+      <c r="D125" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
-        <v>113</v>
-      </c>
-      <c r="B126">
-        <v>424</v>
+        <v>100</v>
+      </c>
+      <c r="C126" t="s">
+        <v>8</v>
+      </c>
+      <c r="D126" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
-        <v>116</v>
-      </c>
-      <c r="B127" t="s">
-        <v>2</v>
+        <v>101</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B128" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
-        <v>120</v>
-      </c>
-      <c r="B129" t="s">
-        <v>121</v>
+        <v>106</v>
+      </c>
+      <c r="B129">
+        <v>424</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B130" t="s">
         <v>2</v>
@@ -2600,248 +2606,282 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B131" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B132" t="s">
-        <v>187</v>
+        <v>114</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>115</v>
+      </c>
+      <c r="B133" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="B134" t="s">
-        <v>138</v>
-      </c>
-      <c r="C134" t="s">
-        <v>141</v>
-      </c>
-      <c r="D134" t="s">
-        <v>134</v>
-      </c>
-      <c r="E134" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A135" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="B135" t="s">
-        <v>143</v>
-      </c>
-      <c r="C135" t="s">
-        <v>141</v>
-      </c>
-      <c r="D135" t="s">
-        <v>134</v>
-      </c>
-      <c r="E135" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A136" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A137" t="s">
-        <v>147</v>
+        <v>125</v>
+      </c>
+      <c r="B137" t="s">
+        <v>131</v>
+      </c>
+      <c r="C137" t="s">
+        <v>134</v>
+      </c>
+      <c r="D137" t="s">
+        <v>127</v>
+      </c>
+      <c r="E137" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A138" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B138" t="s">
-        <v>188</v>
+        <v>136</v>
       </c>
       <c r="C138" t="s">
-        <v>189</v>
+        <v>134</v>
       </c>
       <c r="D138" t="s">
-        <v>190</v>
+        <v>127</v>
       </c>
       <c r="E138" t="s">
-        <v>191</v>
+        <v>135</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A139" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
-        <v>155</v>
+        <v>141</v>
+      </c>
+      <c r="B141" t="s">
+        <v>180</v>
+      </c>
+      <c r="C141" t="s">
+        <v>181</v>
+      </c>
+      <c r="D141" t="s">
+        <v>182</v>
+      </c>
+      <c r="E141" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
-        <v>192</v>
+        <v>146</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A143" t="s">
-        <v>193</v>
+        <v>147</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A144" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A145" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A146" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A147" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A148" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A149" t="s">
-        <v>163</v>
-      </c>
-      <c r="B149" t="s">
-        <v>51</v>
-      </c>
-      <c r="C149" t="s">
-        <v>52</v>
-      </c>
-      <c r="D149" t="s">
-        <v>53</v>
+        <v>153</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A150" t="s">
-        <v>164</v>
-      </c>
-      <c r="B150" t="s">
-        <v>47</v>
-      </c>
-      <c r="C150" t="s">
-        <v>48</v>
-      </c>
-      <c r="D150" t="s">
-        <v>49</v>
+        <v>154</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A151" t="s">
-        <v>165</v>
-      </c>
-      <c r="B151" t="s">
-        <v>55</v>
-      </c>
-      <c r="C151" t="s">
-        <v>56</v>
-      </c>
-      <c r="D151" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A152" t="s">
-        <v>166</v>
+        <v>156</v>
+      </c>
+      <c r="B152" t="s">
+        <v>48</v>
+      </c>
+      <c r="C152" t="s">
+        <v>49</v>
+      </c>
+      <c r="D152" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A153" t="s">
-        <v>167</v>
+        <v>157</v>
+      </c>
+      <c r="B153" t="s">
+        <v>44</v>
+      </c>
+      <c r="C153" t="s">
+        <v>45</v>
+      </c>
+      <c r="D153" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A154" t="s">
-        <v>168</v>
+        <v>158</v>
+      </c>
+      <c r="B154" t="s">
+        <v>52</v>
+      </c>
+      <c r="C154" t="s">
+        <v>53</v>
+      </c>
+      <c r="D154" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A155" t="s">
-        <v>169</v>
-      </c>
-      <c r="B155" t="s">
-        <v>62</v>
-      </c>
-      <c r="C155" t="s">
-        <v>62</v>
-      </c>
-      <c r="D155" t="s">
-        <v>62</v>
+        <v>159</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A156" t="s">
-        <v>170</v>
-      </c>
-      <c r="B156" t="s">
-        <v>64</v>
-      </c>
-      <c r="C156" t="s">
-        <v>64</v>
-      </c>
-      <c r="D156" t="s">
-        <v>64</v>
+        <v>160</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A157" t="s">
-        <v>171</v>
-      </c>
-      <c r="B157" t="s">
-        <v>66</v>
-      </c>
-      <c r="C157" t="s">
-        <v>67</v>
-      </c>
-      <c r="D157" t="s">
-        <v>67</v>
+        <v>161</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A158" t="s">
-        <v>172</v>
+        <v>162</v>
+      </c>
+      <c r="B158" t="s">
+        <v>59</v>
+      </c>
+      <c r="C158" t="s">
+        <v>59</v>
+      </c>
+      <c r="D158" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A159" t="s">
-        <v>173</v>
+        <v>163</v>
+      </c>
+      <c r="B159" t="s">
+        <v>61</v>
+      </c>
+      <c r="C159" t="s">
+        <v>61</v>
+      </c>
+      <c r="D159" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A160" t="s">
-        <v>174</v>
+        <v>164</v>
+      </c>
+      <c r="B160" t="s">
+        <v>63</v>
+      </c>
+      <c r="C160" t="s">
+        <v>64</v>
+      </c>
+      <c r="D160" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A161" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A162" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A163" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A164" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A165" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start reworking assay tests
</commit_message>
<xml_diff>
--- a/tests/ArcCommander.Tests.NetCore/ArcCommander/TestFiles/isa.investigation.xlsx
+++ b/tests/ArcCommander.Tests.NetCore/ArcCommander/TestFiles/isa.investigation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\arcCommander\tests\ArcCommander.Tests.NetCore\ArcCommander\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\ARC_tools\arcCommander\tests\ArcCommander.Tests.NetCore\ArcCommander\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6020251A-48AB-43C8-A088-7EA533E0582E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{685941D2-9566-4014-859A-6AD625F92413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="4230" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Text Document" sheetId="1" r:id="rId1"/>
@@ -258,9 +258,6 @@
     <t>Study File Name</t>
   </si>
   <si>
-    <t>s_BII-S-1.txt</t>
-  </si>
-  <si>
     <t>STUDY DESIGN DESCRIPTORS</t>
   </si>
   <si>
@@ -390,15 +387,6 @@
     <t>Study Assay File Name</t>
   </si>
   <si>
-    <t>a_proteome.txt</t>
-  </si>
-  <si>
-    <t>a_metabolome.txt</t>
-  </si>
-  <si>
-    <t>a_transcriptome.txt</t>
-  </si>
-  <si>
     <t>STUDY PROTOCOLS</t>
   </si>
   <si>
@@ -537,9 +525,6 @@
     <t>Comprehensive high-throughput analyses at the levels of mRNAs, proteins, and metabolites, and studies on gene expression patterns are required for systems biology studies of cell growth [4,26-29]. Although such comprehensive data sets are lacking, many studies have pointed to a central role for the target-of-rapamycin (TOR) signal transduction pathway in growth control. TOR is a serine/threonine kinase that has been conserved from yeasts to mammals; it integrates signals from nutrients or growth factors to regulate cell growth and cell-cycle progression coordinately. Although such comprehensive data sets are lacking, many studies have pointed to a central role for the target-of-rapamycin (TOR) signal transduction pathway in growth control. TOR is a serine/threonine kinase that has been conserved from yeasts to mammals; it integrates signals from nutrients or growth factors to regulate cell growth and cell-cycle progression coordinately. The effect of rapamycin were studied as follows: a culture growing at mid-exponential phase was divided into two. Rapamycin (200 ng/ml) was added to one half, and the drug's solvent to the other, as the control. Samples were taken at 0, 1, 2 and 4 h after treatment. Gene expression at the mRNA level was investigated by transcriptome analysis using Affymetrix hybridization arrays.</t>
   </si>
   <si>
-    <t>s_BII-S-2.txt</t>
-  </si>
-  <si>
     <t>time series design</t>
   </si>
   <si>
@@ -564,9 +549,6 @@
     <t>http://www.ebi.ac.uk/efo/EFO_0000428</t>
   </si>
   <si>
-    <t>a_microarray.txt</t>
-  </si>
-  <si>
     <t>For each target, a hybridisation cocktail was made using the standard array recipe as described in the GeneChip Expression Analysis technical manual. GeneChip control oligonucleotide and 20x eukaryotic hybridisation controls were used. Hybridisation buffer was made as detailed in the GeneChip manual and the BSA and herring sperm DNA was purchased from Invitrogen. The cocktail was heated to 99 C for 5mins, transferred to 45 C for 5 min and then spun for 5 min to remove any insoluble material. Affymetrix Yeast Yg_s98 S. cerevisiae arrays were pre-hybridised with 200 l 1x hybridisation buffer and incubated at 45 C for 10 min. 200 l of the hybridisation cocktail was loaded onto the arrays. The probe array was incubated in a rotisserie at 45 C, rotating at 60 rpm. Following hybridisation, for 16hr, chips were loaded onto a Fluidics station for washing and staining using the EukGe WS2v4 programme controlled using Microarray Suite 5 software.</t>
   </si>
   <si>
@@ -622,6 +604,24 @@
   </si>
   <si>
     <t>Study Publication PubMed ID</t>
+  </si>
+  <si>
+    <t>assays/a_proteome/isa.assay.xlsx</t>
+  </si>
+  <si>
+    <t>assays/a_metabalome/isa.assay.xlsx</t>
+  </si>
+  <si>
+    <t>assays/a_transcriptome/isa.assay.xlsx</t>
+  </si>
+  <si>
+    <t>studies/s_BII-S-1/isa.study.xlsx</t>
+  </si>
+  <si>
+    <t>studies/s_BII-S-2/isa.study.xlsx</t>
+  </si>
+  <si>
+    <t>assays/a_microarray/isa.assay.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1110,48 +1110,48 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1167,7 +1167,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1465,21 +1465,24 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.53515625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1505,12 +1508,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1547,7 +1550,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1573,12 +1576,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1586,7 +1589,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1594,7 +1597,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1602,7 +1605,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1610,7 +1613,7 @@
         <v>2007-04-30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1618,33 +1621,33 @@
         <v>2009-03-10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B16">
         <v>17439666</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1652,7 +1655,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1668,7 +1671,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1676,22 +1679,22 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1705,7 +1708,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1733,22 +1736,22 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1762,7 +1765,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -1776,7 +1779,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -1790,27 +1793,27 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>68</v>
       </c>
@@ -1818,7 +1821,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -1826,7 +1829,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -1834,7 +1837,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>74</v>
       </c>
@@ -1842,7 +1845,7 @@
         <v>2007-04-30</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -1850,192 +1853,192 @@
         <v>2009-03-10</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>76</v>
       </c>
       <c r="B42" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
         <v>79</v>
       </c>
-      <c r="B46" t="s">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
         <v>81</v>
       </c>
-      <c r="B48" t="s">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
-        <v>83</v>
       </c>
       <c r="B49" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B51">
         <v>17439666</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B53" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B54" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" t="s">
         <v>88</v>
       </c>
-      <c r="B55" t="s">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
+      <c r="B59" t="s">
         <v>93</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>94</v>
       </c>
-      <c r="C59" t="s">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A60" t="s">
+      <c r="B60" t="s">
         <v>96</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>97</v>
       </c>
-      <c r="C60" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A61" t="s">
+      <c r="C61" t="s">
         <v>98</v>
       </c>
-      <c r="C61" t="s">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
-        <v>100</v>
       </c>
       <c r="C62" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A64" t="s">
+      <c r="B64" t="s">
         <v>102</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>103</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>104</v>
       </c>
-      <c r="D64" t="s">
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
+      <c r="B65" t="s">
         <v>106</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>107</v>
-      </c>
-      <c r="C65" t="s">
-        <v>108</v>
       </c>
       <c r="D65">
         <v>424</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B66" t="s">
         <v>2</v>
@@ -2047,31 +2050,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>109</v>
+      </c>
+      <c r="B67" t="s">
         <v>110</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" t="s">
         <v>111</v>
       </c>
-      <c r="C67" t="s">
-        <v>111</v>
-      </c>
-      <c r="D67" t="s">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A68" t="s">
+      <c r="D68" t="s">
         <v>113</v>
       </c>
-      <c r="D68" t="s">
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A69" t="s">
-        <v>115</v>
       </c>
       <c r="B69" t="s">
         <v>2</v>
@@ -2083,186 +2086,186 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>115</v>
+      </c>
+      <c r="B70" t="s">
         <v>116</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>117</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>118</v>
       </c>
-      <c r="D70" t="s">
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A71" t="s">
+      <c r="B71" t="s">
+        <v>193</v>
+      </c>
+      <c r="C71" t="s">
+        <v>194</v>
+      </c>
+      <c r="D71" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>120</v>
       </c>
-      <c r="B71" t="s">
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>121</v>
       </c>
-      <c r="C71" t="s">
+      <c r="B73" t="s">
         <v>122</v>
       </c>
-      <c r="D71" t="s">
+      <c r="C73" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A72" t="s">
+      <c r="D73" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A73" t="s">
+      <c r="E73" t="s">
         <v>125</v>
       </c>
-      <c r="B73" t="s">
+      <c r="F73" t="s">
         <v>126</v>
       </c>
-      <c r="C73" t="s">
+      <c r="G73" t="s">
         <v>127</v>
       </c>
-      <c r="D73" t="s">
+      <c r="H73" t="s">
         <v>128</v>
       </c>
-      <c r="E73" t="s">
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>129</v>
       </c>
-      <c r="F73" t="s">
+      <c r="B74" t="s">
         <v>130</v>
       </c>
-      <c r="G73" t="s">
+      <c r="C74" t="s">
+        <v>123</v>
+      </c>
+      <c r="D74" t="s">
+        <v>124</v>
+      </c>
+      <c r="E74" t="s">
         <v>131</v>
       </c>
-      <c r="H73" t="s">
+      <c r="F74" t="s">
+        <v>131</v>
+      </c>
+      <c r="G74" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A74" t="s">
+      <c r="H74" t="s">
         <v>133</v>
       </c>
-      <c r="B74" t="s">
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>134</v>
       </c>
-      <c r="C74" t="s">
-        <v>127</v>
-      </c>
-      <c r="D74" t="s">
-        <v>128</v>
-      </c>
-      <c r="E74" t="s">
+      <c r="H75" t="s">
         <v>135</v>
       </c>
-      <c r="F74" t="s">
-        <v>135</v>
-      </c>
-      <c r="G74" t="s">
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>136</v>
-      </c>
-      <c r="H74" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A75" t="s">
-        <v>138</v>
-      </c>
-      <c r="H75" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A76" t="s">
-        <v>140</v>
       </c>
       <c r="H76" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>137</v>
+      </c>
+      <c r="B77" t="s">
+        <v>138</v>
+      </c>
+      <c r="C77" t="s">
+        <v>139</v>
+      </c>
+      <c r="E77" t="s">
+        <v>140</v>
+      </c>
+      <c r="G77" t="s">
         <v>141</v>
       </c>
-      <c r="B77" t="s">
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>142</v>
       </c>
-      <c r="C77" t="s">
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>143</v>
       </c>
-      <c r="E77" t="s">
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>144</v>
       </c>
-      <c r="G77" t="s">
+      <c r="H80" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A78" t="s">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>178</v>
+      </c>
+      <c r="H81" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A79" t="s">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>179</v>
+      </c>
+      <c r="H82" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A80" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>148</v>
       </c>
-      <c r="H80" t="s">
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A81" t="s">
-        <v>184</v>
-      </c>
-      <c r="H81" t="s">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A82" t="s">
-        <v>185</v>
-      </c>
-      <c r="H82" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A83" t="s">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A84" t="s">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A85" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A86" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A87" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A88" t="s">
-        <v>156</v>
       </c>
       <c r="B88" t="s">
         <v>48</v>
@@ -2274,9 +2277,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B89" t="s">
         <v>44</v>
@@ -2288,9 +2291,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B90" t="s">
         <v>52</v>
@@ -2302,24 +2305,24 @@
         <v>54</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B94" t="s">
         <v>59</v>
@@ -2331,9 +2334,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B95" t="s">
         <v>61</v>
@@ -2345,9 +2348,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B96" t="s">
         <v>63</v>
@@ -2359,56 +2362,56 @@
         <v>64</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.4">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.4">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>68</v>
       </c>
       <c r="B102" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.4">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>70</v>
       </c>
       <c r="B103" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.4">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>72</v>
       </c>
       <c r="B104" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>74</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>2007-04-30</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>75</v>
       </c>
@@ -2424,149 +2427,149 @@
         <v>2009-03-10</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>76</v>
       </c>
       <c r="B107" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.4">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.4">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A111" t="s">
-        <v>79</v>
-      </c>
       <c r="B111" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B112" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.4">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B113" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B115">
         <v>17439666</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A117" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A118" t="s">
-        <v>87</v>
       </c>
       <c r="B118" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B119" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A121" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A122" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A123" t="s">
-        <v>93</v>
-      </c>
       <c r="B123" t="s">
+        <v>168</v>
+      </c>
+      <c r="C123" t="s">
+        <v>169</v>
+      </c>
+      <c r="D123" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>95</v>
+      </c>
+      <c r="B124" t="s">
+        <v>168</v>
+      </c>
+      <c r="C124" t="s">
+        <v>171</v>
+      </c>
+      <c r="D124" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>97</v>
+      </c>
+      <c r="C125" t="s">
+        <v>172</v>
+      </c>
+      <c r="D125" t="s">
         <v>173</v>
       </c>
-      <c r="C123" t="s">
-        <v>174</v>
-      </c>
-      <c r="D123" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A124" t="s">
-        <v>96</v>
-      </c>
-      <c r="B124" t="s">
-        <v>173</v>
-      </c>
-      <c r="C124" t="s">
-        <v>176</v>
-      </c>
-      <c r="D124" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A125" t="s">
-        <v>98</v>
-      </c>
-      <c r="C125" t="s">
-        <v>177</v>
-      </c>
-      <c r="D125" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.4">
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C126" t="s">
         <v>8</v>
@@ -2575,194 +2578,194 @@
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A128" t="s">
-        <v>102</v>
-      </c>
       <c r="B128" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A129" t="s">
-        <v>106</v>
       </c>
       <c r="B129">
         <v>424</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B130" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B131" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A132" t="s">
+      <c r="B132" t="s">
         <v>113</v>
       </c>
-      <c r="B132" t="s">
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A133" t="s">
-        <v>115</v>
       </c>
       <c r="B133" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B134" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A135" t="s">
+      <c r="B135" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>120</v>
       </c>
-      <c r="B135" t="s">
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>121</v>
+      </c>
+      <c r="B137" t="s">
+        <v>127</v>
+      </c>
+      <c r="C137" t="s">
+        <v>130</v>
+      </c>
+      <c r="D137" t="s">
+        <v>123</v>
+      </c>
+      <c r="E137" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>129</v>
+      </c>
+      <c r="B138" t="s">
+        <v>132</v>
+      </c>
+      <c r="C138" t="s">
+        <v>130</v>
+      </c>
+      <c r="D138" t="s">
+        <v>123</v>
+      </c>
+      <c r="E138" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>137</v>
+      </c>
+      <c r="B141" t="s">
+        <v>174</v>
+      </c>
+      <c r="C141" t="s">
+        <v>175</v>
+      </c>
+      <c r="D141" t="s">
+        <v>176</v>
+      </c>
+      <c r="E141" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A136" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A137" t="s">
-        <v>125</v>
-      </c>
-      <c r="B137" t="s">
-        <v>131</v>
-      </c>
-      <c r="C137" t="s">
-        <v>134</v>
-      </c>
-      <c r="D137" t="s">
-        <v>127</v>
-      </c>
-      <c r="E137" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A138" t="s">
-        <v>133</v>
-      </c>
-      <c r="B138" t="s">
-        <v>136</v>
-      </c>
-      <c r="C138" t="s">
-        <v>134</v>
-      </c>
-      <c r="D138" t="s">
-        <v>127</v>
-      </c>
-      <c r="E138" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A139" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A140" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A141" t="s">
-        <v>141</v>
-      </c>
-      <c r="B141" t="s">
-        <v>180</v>
-      </c>
-      <c r="C141" t="s">
-        <v>181</v>
-      </c>
-      <c r="D141" t="s">
-        <v>182</v>
-      </c>
-      <c r="E141" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A142" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A143" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A144" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A145" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A146" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A147" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A148" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A149" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A150" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A151" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A152" t="s">
-        <v>156</v>
       </c>
       <c r="B152" t="s">
         <v>48</v>
@@ -2774,9 +2777,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B153" t="s">
         <v>44</v>
@@ -2788,9 +2791,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B154" t="s">
         <v>52</v>
@@ -2802,24 +2805,24 @@
         <v>54</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.4">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.4">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.4">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B158" t="s">
         <v>59</v>
@@ -2831,9 +2834,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B159" t="s">
         <v>61</v>
@@ -2845,9 +2848,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B160" t="s">
         <v>63</v>
@@ -2859,29 +2862,29 @@
         <v>64</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.4">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.4">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>